<commit_message>
Adjustments for all short links
</commit_message>
<xml_diff>
--- a/Endnotes/archive/DEBP Master.gitnote.xlsx
+++ b/Endnotes/archive/DEBP Master.gitnote.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa_000\Documents\gitnotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa_000\Documents\Data-Engineering-Best-Practices\Endnotes\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D39A6-AD90-4807-A0A0-11FA4A964C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601FAFB6-5D4B-4A4C-BC83-7A1161D63CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{8D3C63F4-5A6B-43ED-8FE0-3091290B56A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8D3C63F4-5A6B-43ED-8FE0-3091290B56A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Links" sheetId="16" r:id="rId1"/>
+    <sheet name="Summary" sheetId="16" r:id="rId1"/>
     <sheet name="chapter-1" sheetId="2" r:id="rId2"/>
     <sheet name="chapter-2" sheetId="3" r:id="rId3"/>
     <sheet name="chapter-3" sheetId="4" r:id="rId4"/>
@@ -24,8 +24,8 @@
     <sheet name="chapter-8" sheetId="9" r:id="rId9"/>
     <sheet name="chapter-9" sheetId="10" r:id="rId10"/>
     <sheet name="chapter-10" sheetId="11" r:id="rId11"/>
-    <sheet name="chapter-12" sheetId="13" r:id="rId12"/>
-    <sheet name="chapter-11" sheetId="12" r:id="rId13"/>
+    <sheet name="chapter-11" sheetId="12" r:id="rId12"/>
+    <sheet name="chapter-12" sheetId="13" r:id="rId13"/>
     <sheet name="chapter-13" sheetId="1" r:id="rId14"/>
     <sheet name="chapter-14" sheetId="14" r:id="rId15"/>
     <sheet name="chapter-15" sheetId="15" r:id="rId16"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="11">
   <si>
     <t>DEBP ENDNOTE CHAPTER</t>
   </si>
@@ -80,598 +80,13 @@
     <t>#</t>
   </si>
   <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/65.htm</t>
+    <t>Chapter</t>
   </si>
   <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #65</t>
+    <t># Links</t>
   </si>
   <si>
-    <t>https://packt-debp.link/eazkXZ</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/64.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #64</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/PGDfAt</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/63.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #63</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/mn0jUI</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/62.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #62</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/K3ac1Q</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/61.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #61</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Hga7zE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/60.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #60</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/IwW2go</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/59.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #59</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/9LOiCu</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/58.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #58</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/IZbU9n</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/57.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #57</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/XvBucF</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/56.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #56</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/XjJKxz</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/55.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #55</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/t8BSf3</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/54.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #54</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/aFa7TS</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/53.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #53</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DkijVm</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/52.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #52</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/o5cAnA</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/51.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #51</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/SOGmGK</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/50.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #50</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/xr84Ct</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/49.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #49</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jGGFrx</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/48.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #48</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/2Ud8O7</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/47.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #47</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/qVhsHe</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/46.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #46</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/7QTtB2</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/45.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #45</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/nclKxX</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/44.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #44</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/oJRDVR</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/43.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #43</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Gec8uH</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/42.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #42</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DFoVOe</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/41.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #41</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Rft3K5</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/40.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #40</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/9teCPO</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/39.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #39</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/MqRT1r</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/38.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #38</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DAdKBy</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/37.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #37</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/aD5xk2</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/36.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #36</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/ArgUFg</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/35.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #35</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/BAricy</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/34.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #34</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/JTUbkg</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/33.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #33</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DIJwXL</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/32.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #32</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/6hIVq0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/31.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #31</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/sp4re9</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/30.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #30</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/haDtM0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/29.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #29</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/oukXsc</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/28.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #28</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/mRPViY</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/27.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #27</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/RdluoB</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/26.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #26</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/kjaH7P</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/25.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #25</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/YMZ0ZE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/24.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #24</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/3UbXmd</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/23.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #23</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/PgXjAQ</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/22.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #22</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/lSxGyj</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/21.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #21</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/KjSXa7</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/20.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #20</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/n2Napt</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/19.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #19</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/nxA1f5</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/18.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #18</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jkmbnM</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/17.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #17</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/WoybzT</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/16.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #16</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OtxSUz</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/15.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #15</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/ca3osh</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/14.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #14</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/5F2597</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/13.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #13</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jC1mU6</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/12.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #12</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/JZv09V</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/11.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #11</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/r7TVfq</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/10.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #10</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/isW81S</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/9.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #9</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/wFFwaM</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/8.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #8</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/sWMfn0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/7.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #7</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/seyIN4</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/6.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #6</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OoN2s3</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/5.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #5</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/0TvCOE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/4.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #4</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/qBSMA6</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/3.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #3</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/SHc96l</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/2.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #2</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/dZ7j9f</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/1.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #1</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OUgn3l</t>
-  </si>
-  <si>
-    <t>Original URL</t>
-  </si>
-  <si>
-    <t>Link title</t>
-  </si>
-  <si>
-    <t>Short link</t>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -726,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,9 +157,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1082,942 +494,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E062FD-AFB8-4151-84F1-25E3FF36BC8B}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="98.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="B8" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="B11" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="B12" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="B13" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="B14" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="B15" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="B16" s="6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="6">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
+      <c r="B19" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
-        <v>56</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
-        <v>57</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
-        <v>58</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="7">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
-        <v>62</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
-        <v>63</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
-        <v>64</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="7">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>8</v>
+      <c r="B20" s="6">
+        <f>SUM(B2:B19)</f>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -2030,7 +681,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,7 +834,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,11 +1163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99018CC5-B0B1-4FED-AD8A-1B39DD310BB3}">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA82E97-AF44-40FB-A7F7-EAEC05C1A9A0}">
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B71"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2573,7 +1224,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B65" ca="1" si="0">CONCATENATE($B$1," ", $J$1, " #", $A2, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A2, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 12 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/1.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/1.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2583,7 +1234,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/2.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/2.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2593,7 +1244,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/3.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/3.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2603,7 +1254,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/4.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/4.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,7 +1264,7 @@
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/5.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/5.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2623,7 +1274,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/6.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/6.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2633,7 +1284,7 @@
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/7.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/7.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2643,7 +1294,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/8.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/8.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2653,7 +1304,7 @@
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/9.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/9.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2663,7 +1314,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/10.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/10.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,7 +1324,7 @@
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/11.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/11.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2683,7 +1334,7 @@
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/12.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/12.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2693,7 +1344,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/13.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/13.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2703,7 +1354,7 @@
       </c>
       <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/14.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/14.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2713,7 +1364,7 @@
       </c>
       <c r="B16" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/15.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/15.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +1374,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/16.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/16.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2733,7 +1384,7 @@
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/17.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/17.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2743,7 +1394,7 @@
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/18.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/18.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2753,7 +1404,7 @@
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/19.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/19.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,7 +1414,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/20.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/20.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2773,7 +1424,7 @@
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/21.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/21.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,7 +1434,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/22.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/22.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2793,7 +1444,7 @@
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/23.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/23.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2803,7 +1454,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/24.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/24.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,7 +1464,7 @@
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/25.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/25.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2823,7 +1474,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/26.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/26.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2833,7 +1484,7 @@
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/27.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/27.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2843,7 +1494,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/28.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/28.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2853,7 +1504,7 @@
       </c>
       <c r="B30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/29.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/29.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2863,7 +1514,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/30.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/30.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2873,7 +1524,7 @@
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/31.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/31.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2883,7 +1534,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/32.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/32.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2893,7 +1544,7 @@
       </c>
       <c r="B34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/33.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/33.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2903,7 +1554,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/34.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/34.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,7 +1564,7 @@
       </c>
       <c r="B36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/35.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/35.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2923,7 +1574,7 @@
       </c>
       <c r="B37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/36.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/36.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,7 +1584,7 @@
       </c>
       <c r="B38" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/37.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/37.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2943,7 +1594,7 @@
       </c>
       <c r="B39" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/38.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/38.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2953,7 +1604,7 @@
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/39.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/39.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2963,7 +1614,7 @@
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/40.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/40.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,7 +1624,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/41.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/41.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2983,7 +1634,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/42.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/42.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2993,7 +1644,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/43.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/43.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3003,7 +1654,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/44.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/44.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3013,7 +1664,7 @@
       </c>
       <c r="B46" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/45.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/45.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3023,7 +1674,7 @@
       </c>
       <c r="B47" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/46.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/46.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3033,7 +1684,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/47.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/47.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,7 +1694,7 @@
       </c>
       <c r="B49" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/48.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/48.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3053,7 +1704,7 @@
       </c>
       <c r="B50" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/49.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/49.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3063,7 +1714,7 @@
       </c>
       <c r="B51" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/50.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/50.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3073,7 +1724,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/51.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/51.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3083,7 +1734,7 @@
       </c>
       <c r="B53" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/52.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/52.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3093,7 +1744,7 @@
       </c>
       <c r="B54" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/53.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/53.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3103,7 +1754,7 @@
       </c>
       <c r="B55" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/54.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/54.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3113,7 +1764,7 @@
       </c>
       <c r="B56" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/55.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/55.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3123,7 +1774,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/56.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/56.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3133,7 +1784,7 @@
       </c>
       <c r="B58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/57.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/57.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3143,7 +1794,7 @@
       </c>
       <c r="B59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/58.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/58.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3153,7 +1804,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/59.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/59.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3163,7 +1814,7 @@
       </c>
       <c r="B61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/60.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/60.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,7 +1824,7 @@
       </c>
       <c r="B62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/61.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/61.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3183,7 +1834,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/62.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/62.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3193,7 +1844,7 @@
       </c>
       <c r="B64" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/63.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/63.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3203,7 +1854,7 @@
       </c>
       <c r="B65" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/64.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/64.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,8 +1863,8 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" ref="B66:B71" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 12 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/65.htm,pack-debp-chapter-12</v>
+        <f t="shared" ref="B66:B74" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
+        <v>DEBP ENDNOTE CHAPTER 11 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/65.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3223,17 +1874,17 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/66.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/66.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A71" si="3">A67+1</f>
+        <f t="shared" ref="A68:A74" si="3">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/67.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/67.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3243,7 +1894,7 @@
       </c>
       <c r="B69" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/68.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/68.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3253,7 +1904,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/69.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/69.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,23 +1914,53 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/70.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/70.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #71,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/71.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #72,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/72.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #73,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/73.htm,pack-debp-chapter-11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{16425970-E582-43CF-965B-9386FA682BEF}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{68968D13-14DC-481C-A53E-F0199DD9C6CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA82E97-AF44-40FB-A7F7-EAEC05C1A9A0}">
-  <dimension ref="A1:J74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99018CC5-B0B1-4FED-AD8A-1B39DD310BB3}">
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B74"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,7 +2008,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3336,7 +2017,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B65" ca="1" si="0">CONCATENATE($B$1," ", $J$1, " #", $A2, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A2, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 11 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/1.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/1.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3346,7 +2027,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/2.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/2.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3356,7 +2037,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/3.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/3.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3366,7 +2047,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/4.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/4.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3376,7 +2057,7 @@
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/5.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/5.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3386,7 +2067,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/6.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/6.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3396,7 +2077,7 @@
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/7.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/7.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3406,7 +2087,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/8.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/8.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3416,7 +2097,7 @@
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/9.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/9.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3426,7 +2107,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/10.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/10.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3436,7 +2117,7 @@
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/11.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/11.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3446,7 +2127,7 @@
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/12.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/12.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3456,7 +2137,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/13.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/13.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3466,7 +2147,7 @@
       </c>
       <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/14.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/14.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3476,7 +2157,7 @@
       </c>
       <c r="B16" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/15.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/15.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3486,7 +2167,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/16.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/16.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,7 +2177,7 @@
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/17.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/17.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3506,7 +2187,7 @@
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/18.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/18.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3516,7 +2197,7 @@
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/19.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/19.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3526,7 +2207,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/20.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/20.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3536,7 +2217,7 @@
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/21.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/21.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3546,7 +2227,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/22.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/22.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3556,7 +2237,7 @@
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/23.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/23.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3566,7 +2247,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/24.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/24.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,7 +2257,7 @@
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/25.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/25.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3586,7 +2267,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/26.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/26.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3596,7 +2277,7 @@
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/27.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/27.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3606,7 +2287,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/28.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/28.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3616,7 +2297,7 @@
       </c>
       <c r="B30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/29.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/29.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3626,7 +2307,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/30.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/30.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3636,7 +2317,7 @@
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/31.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/31.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3646,7 +2327,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/32.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/32.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3656,7 +2337,7 @@
       </c>
       <c r="B34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/33.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/33.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3666,7 +2347,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/34.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/34.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3676,7 +2357,7 @@
       </c>
       <c r="B36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/35.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/35.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3686,7 +2367,7 @@
       </c>
       <c r="B37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/36.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/36.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3696,7 +2377,7 @@
       </c>
       <c r="B38" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/37.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/37.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3706,7 +2387,7 @@
       </c>
       <c r="B39" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/38.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/38.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3716,7 +2397,7 @@
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/39.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/39.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3726,7 +2407,7 @@
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/40.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/40.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3736,7 +2417,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/41.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/41.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3746,7 +2427,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/42.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/42.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3756,7 +2437,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/43.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/43.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3766,7 +2447,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/44.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/44.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3776,7 +2457,7 @@
       </c>
       <c r="B46" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/45.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/45.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3786,7 +2467,7 @@
       </c>
       <c r="B47" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/46.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/46.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3796,7 +2477,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/47.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/47.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3806,7 +2487,7 @@
       </c>
       <c r="B49" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/48.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/48.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3816,7 +2497,7 @@
       </c>
       <c r="B50" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/49.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/49.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3826,7 +2507,7 @@
       </c>
       <c r="B51" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/50.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/50.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3836,7 +2517,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/51.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/51.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3846,7 +2527,7 @@
       </c>
       <c r="B53" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/52.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/52.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3856,7 +2537,7 @@
       </c>
       <c r="B54" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/53.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/53.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3866,7 +2547,7 @@
       </c>
       <c r="B55" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/54.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/54.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3876,7 +2557,7 @@
       </c>
       <c r="B56" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/55.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/55.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3886,7 +2567,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/56.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/56.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3896,7 +2577,7 @@
       </c>
       <c r="B58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/57.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/57.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3906,7 +2587,7 @@
       </c>
       <c r="B59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/58.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/58.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3916,7 +2597,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/59.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/59.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +2607,7 @@
       </c>
       <c r="B61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/60.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/60.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3936,7 +2617,7 @@
       </c>
       <c r="B62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/61.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/61.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3946,7 +2627,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/62.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/62.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3956,7 +2637,7 @@
       </c>
       <c r="B64" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/63.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/63.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,7 +2647,7 @@
       </c>
       <c r="B65" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/64.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/64.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3975,8 +2656,8 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" ref="B66:B74" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 11 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/65.htm,pack-debp-chapter-11</v>
+        <f t="shared" ref="B66:B71" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
+        <v>DEBP ENDNOTE CHAPTER 12 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/65.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3986,17 +2667,17 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/66.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/66.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A74" si="3">A67+1</f>
+        <f t="shared" ref="A68:A71" si="3">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/67.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/67.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -4006,7 +2687,7 @@
       </c>
       <c r="B69" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/68.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/68.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -4016,7 +2697,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/69.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/69.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -4026,42 +2707,12 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/70.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="B72" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #71,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/71.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="B73" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #72,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/72.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B74" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #73,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/73.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/70.htm,pack-debp-chapter-12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{68968D13-14DC-481C-A53E-F0199DD9C6CD}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{16425970-E582-43CF-965B-9386FA682BEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4071,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C499C072-DED7-4062-8960-4AF5EC3C5A22}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4785,7 +3436,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B78"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8800,7 +7451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BFB414-1A9D-4ADF-BFBB-0A684113C784}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -8923,8 +7574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E26A37-2E30-42BA-A1DF-2E467DE615AC}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9997,7 +8648,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B57"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12549,7 +11200,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B57"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adjusted Summary.  THere are 1012 links in this book
</commit_message>
<xml_diff>
--- a/Endnotes/archive/DEBP Master.gitnote.xlsx
+++ b/Endnotes/archive/DEBP Master.gitnote.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa_000\Documents\gitnotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa_000\Documents\Data-Engineering-Best-Practices\Endnotes\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D39A6-AD90-4807-A0A0-11FA4A964C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601FAFB6-5D4B-4A4C-BC83-7A1161D63CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{8D3C63F4-5A6B-43ED-8FE0-3091290B56A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8D3C63F4-5A6B-43ED-8FE0-3091290B56A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Links" sheetId="16" r:id="rId1"/>
+    <sheet name="Summary" sheetId="16" r:id="rId1"/>
     <sheet name="chapter-1" sheetId="2" r:id="rId2"/>
     <sheet name="chapter-2" sheetId="3" r:id="rId3"/>
     <sheet name="chapter-3" sheetId="4" r:id="rId4"/>
@@ -24,8 +24,8 @@
     <sheet name="chapter-8" sheetId="9" r:id="rId9"/>
     <sheet name="chapter-9" sheetId="10" r:id="rId10"/>
     <sheet name="chapter-10" sheetId="11" r:id="rId11"/>
-    <sheet name="chapter-12" sheetId="13" r:id="rId12"/>
-    <sheet name="chapter-11" sheetId="12" r:id="rId13"/>
+    <sheet name="chapter-11" sheetId="12" r:id="rId12"/>
+    <sheet name="chapter-12" sheetId="13" r:id="rId13"/>
     <sheet name="chapter-13" sheetId="1" r:id="rId14"/>
     <sheet name="chapter-14" sheetId="14" r:id="rId15"/>
     <sheet name="chapter-15" sheetId="15" r:id="rId16"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="11">
   <si>
     <t>DEBP ENDNOTE CHAPTER</t>
   </si>
@@ -80,598 +80,13 @@
     <t>#</t>
   </si>
   <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/65.htm</t>
+    <t>Chapter</t>
   </si>
   <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #65</t>
+    <t># Links</t>
   </si>
   <si>
-    <t>https://packt-debp.link/eazkXZ</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/64.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #64</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/PGDfAt</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/63.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #63</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/mn0jUI</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/62.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #62</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/K3ac1Q</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/61.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #61</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Hga7zE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/60.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #60</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/IwW2go</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/59.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #59</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/9LOiCu</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/58.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #58</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/IZbU9n</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/57.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #57</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/XvBucF</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/56.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #56</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/XjJKxz</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/55.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #55</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/t8BSf3</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/54.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #54</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/aFa7TS</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/53.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #53</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DkijVm</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/52.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #52</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/o5cAnA</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/51.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #51</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/SOGmGK</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/50.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #50</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/xr84Ct</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/49.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #49</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jGGFrx</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/48.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #48</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/2Ud8O7</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/47.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #47</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/qVhsHe</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/46.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #46</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/7QTtB2</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/45.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #45</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/nclKxX</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/44.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #44</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/oJRDVR</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/43.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #43</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Gec8uH</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/42.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #42</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DFoVOe</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/41.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #41</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/Rft3K5</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/40.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #40</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/9teCPO</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/39.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #39</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/MqRT1r</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/38.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #38</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DAdKBy</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/37.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #37</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/aD5xk2</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/36.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #36</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/ArgUFg</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/35.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #35</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/BAricy</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/34.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #34</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/JTUbkg</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/33.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #33</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/DIJwXL</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/32.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #32</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/6hIVq0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/31.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #31</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/sp4re9</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/30.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #30</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/haDtM0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/29.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #29</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/oukXsc</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/28.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #28</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/mRPViY</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/27.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #27</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/RdluoB</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/26.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #26</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/kjaH7P</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/25.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #25</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/YMZ0ZE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/24.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #24</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/3UbXmd</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/23.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #23</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/PgXjAQ</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/22.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #22</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/lSxGyj</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/21.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #21</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/KjSXa7</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/20.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #20</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/n2Napt</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/19.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #19</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/nxA1f5</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/18.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #18</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jkmbnM</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/17.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #17</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/WoybzT</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/16.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #16</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OtxSUz</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/15.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #15</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/ca3osh</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/14.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #14</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/5F2597</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/13.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #13</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/jC1mU6</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/12.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #12</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/JZv09V</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/11.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #11</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/r7TVfq</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/10.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #10</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/isW81S</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/9.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #9</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/wFFwaM</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/8.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #8</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/sWMfn0</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/7.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #7</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/seyIN4</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/6.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #6</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OoN2s3</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/5.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #5</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/0TvCOE</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/4.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #4</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/qBSMA6</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/3.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #3</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/SHc96l</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/2.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #2</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/dZ7j9f</t>
-  </si>
-  <si>
-    <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-13/1.htm</t>
-  </si>
-  <si>
-    <t>DEBP ENDNOTE CHAPTER 13 #1</t>
-  </si>
-  <si>
-    <t>https://packt-debp.link/OUgn3l</t>
-  </si>
-  <si>
-    <t>Original URL</t>
-  </si>
-  <si>
-    <t>Link title</t>
-  </si>
-  <si>
-    <t>Short link</t>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -726,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,9 +157,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1082,942 +494,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E062FD-AFB8-4151-84F1-25E3FF36BC8B}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="98.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="B8" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="B11" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="B12" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="B13" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="B14" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="B15" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="B16" s="6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="6">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
+      <c r="B19" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
-        <v>56</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
-        <v>57</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
-        <v>58</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="7">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
-        <v>62</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
-        <v>63</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
-        <v>64</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="7">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>8</v>
+      <c r="B20" s="6">
+        <f>SUM(B2:B19)</f>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -2030,7 +681,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,7 +834,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,11 +1163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99018CC5-B0B1-4FED-AD8A-1B39DD310BB3}">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA82E97-AF44-40FB-A7F7-EAEC05C1A9A0}">
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B71"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2573,7 +1224,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B65" ca="1" si="0">CONCATENATE($B$1," ", $J$1, " #", $A2, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A2, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 12 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/1.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/1.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2583,7 +1234,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/2.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/2.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2593,7 +1244,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/3.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/3.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2603,7 +1254,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/4.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/4.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,7 +1264,7 @@
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/5.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/5.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2623,7 +1274,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/6.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/6.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2633,7 +1284,7 @@
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/7.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/7.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2643,7 +1294,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/8.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/8.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2653,7 +1304,7 @@
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/9.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/9.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2663,7 +1314,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/10.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/10.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,7 +1324,7 @@
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/11.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/11.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2683,7 +1334,7 @@
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/12.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/12.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2693,7 +1344,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/13.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/13.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2703,7 +1354,7 @@
       </c>
       <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/14.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/14.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2713,7 +1364,7 @@
       </c>
       <c r="B16" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/15.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/15.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +1374,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/16.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/16.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2733,7 +1384,7 @@
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/17.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/17.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2743,7 +1394,7 @@
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/18.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/18.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2753,7 +1404,7 @@
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/19.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/19.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,7 +1414,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/20.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/20.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2773,7 +1424,7 @@
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/21.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/21.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,7 +1434,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/22.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/22.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2793,7 +1444,7 @@
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/23.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/23.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2803,7 +1454,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/24.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/24.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,7 +1464,7 @@
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/25.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/25.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2823,7 +1474,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/26.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/26.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2833,7 +1484,7 @@
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/27.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/27.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2843,7 +1494,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/28.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/28.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2853,7 +1504,7 @@
       </c>
       <c r="B30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/29.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/29.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2863,7 +1514,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/30.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/30.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2873,7 +1524,7 @@
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/31.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/31.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2883,7 +1534,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/32.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/32.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2893,7 +1544,7 @@
       </c>
       <c r="B34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/33.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/33.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2903,7 +1554,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/34.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/34.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,7 +1564,7 @@
       </c>
       <c r="B36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/35.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/35.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2923,7 +1574,7 @@
       </c>
       <c r="B37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/36.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/36.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,7 +1584,7 @@
       </c>
       <c r="B38" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/37.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/37.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2943,7 +1594,7 @@
       </c>
       <c r="B39" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/38.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/38.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2953,7 +1604,7 @@
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/39.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/39.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2963,7 +1614,7 @@
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/40.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/40.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,7 +1624,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/41.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/41.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2983,7 +1634,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/42.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/42.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2993,7 +1644,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/43.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/43.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3003,7 +1654,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/44.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/44.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3013,7 +1664,7 @@
       </c>
       <c r="B46" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/45.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/45.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3023,7 +1674,7 @@
       </c>
       <c r="B47" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/46.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/46.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3033,7 +1684,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/47.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/47.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,7 +1694,7 @@
       </c>
       <c r="B49" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/48.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/48.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3053,7 +1704,7 @@
       </c>
       <c r="B50" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/49.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/49.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3063,7 +1714,7 @@
       </c>
       <c r="B51" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/50.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/50.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3073,7 +1724,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/51.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/51.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3083,7 +1734,7 @@
       </c>
       <c r="B53" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/52.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/52.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3093,7 +1744,7 @@
       </c>
       <c r="B54" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/53.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/53.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3103,7 +1754,7 @@
       </c>
       <c r="B55" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/54.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/54.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3113,7 +1764,7 @@
       </c>
       <c r="B56" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/55.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/55.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3123,7 +1774,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/56.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/56.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3133,7 +1784,7 @@
       </c>
       <c r="B58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/57.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/57.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3143,7 +1794,7 @@
       </c>
       <c r="B59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/58.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/58.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3153,7 +1804,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/59.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/59.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3163,7 +1814,7 @@
       </c>
       <c r="B61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/60.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/60.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,7 +1824,7 @@
       </c>
       <c r="B62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/61.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/61.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3183,7 +1834,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/62.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/62.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3193,7 +1844,7 @@
       </c>
       <c r="B64" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/63.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/63.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3203,7 +1854,7 @@
       </c>
       <c r="B65" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/64.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/64.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,8 +1863,8 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" ref="B66:B71" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 12 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/65.htm,pack-debp-chapter-12</v>
+        <f t="shared" ref="B66:B74" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
+        <v>DEBP ENDNOTE CHAPTER 11 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/65.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3223,17 +1874,17 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/66.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/66.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A71" si="3">A67+1</f>
+        <f t="shared" ref="A68:A74" si="3">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/67.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/67.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3243,7 +1894,7 @@
       </c>
       <c r="B69" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/68.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/68.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3253,7 +1904,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/69.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/69.htm,pack-debp-chapter-11</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,23 +1914,53 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 12 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/70.htm,pack-debp-chapter-12</v>
+        <v>DEBP ENDNOTE CHAPTER 11 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/70.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #71,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/71.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #72,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/72.htm,pack-debp-chapter-11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>DEBP ENDNOTE CHAPTER 11 #73,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/73.htm,pack-debp-chapter-11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{16425970-E582-43CF-965B-9386FA682BEF}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{68968D13-14DC-481C-A53E-F0199DD9C6CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA82E97-AF44-40FB-A7F7-EAEC05C1A9A0}">
-  <dimension ref="A1:J74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99018CC5-B0B1-4FED-AD8A-1B39DD310BB3}">
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B74"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,7 +2008,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3336,7 +2017,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B65" ca="1" si="0">CONCATENATE($B$1," ", $J$1, " #", $A2, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A2, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 11 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/1.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #1,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/1.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3346,7 +2027,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/2.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #2,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/2.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3356,7 +2037,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/3.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #3,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/3.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3366,7 +2047,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/4.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #4,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/4.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3376,7 +2057,7 @@
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/5.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #5,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/5.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3386,7 +2067,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/6.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #6,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/6.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3396,7 +2077,7 @@
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/7.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #7,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/7.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3406,7 +2087,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/8.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #8,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/8.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3416,7 +2097,7 @@
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/9.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #9,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/9.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3426,7 +2107,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/10.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #10,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/10.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3436,7 +2117,7 @@
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/11.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #11,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/11.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3446,7 +2127,7 @@
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/12.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #12,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/12.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3456,7 +2137,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/13.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #13,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/13.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3466,7 +2147,7 @@
       </c>
       <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/14.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #14,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/14.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3476,7 +2157,7 @@
       </c>
       <c r="B16" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/15.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #15,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/15.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3486,7 +2167,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/16.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #16,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/16.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,7 +2177,7 @@
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/17.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #17,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/17.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3506,7 +2187,7 @@
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/18.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #18,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/18.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3516,7 +2197,7 @@
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/19.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #19,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/19.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3526,7 +2207,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/20.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #20,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/20.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3536,7 +2217,7 @@
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/21.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #21,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/21.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3546,7 +2227,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/22.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #22,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/22.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3556,7 +2237,7 @@
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/23.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #23,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/23.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3566,7 +2247,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/24.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #24,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/24.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,7 +2257,7 @@
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/25.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #25,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/25.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3586,7 +2267,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/26.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #26,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/26.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3596,7 +2277,7 @@
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/27.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #27,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/27.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3606,7 +2287,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/28.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #28,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/28.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3616,7 +2297,7 @@
       </c>
       <c r="B30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/29.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #29,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/29.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3626,7 +2307,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/30.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #30,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/30.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3636,7 +2317,7 @@
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/31.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #31,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/31.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3646,7 +2327,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/32.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #32,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/32.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3656,7 +2337,7 @@
       </c>
       <c r="B34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/33.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #33,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/33.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3666,7 +2347,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/34.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #34,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/34.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3676,7 +2357,7 @@
       </c>
       <c r="B36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/35.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #35,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/35.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3686,7 +2367,7 @@
       </c>
       <c r="B37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/36.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #36,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/36.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3696,7 +2377,7 @@
       </c>
       <c r="B38" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/37.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #37,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/37.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3706,7 +2387,7 @@
       </c>
       <c r="B39" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/38.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #38,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/38.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3716,7 +2397,7 @@
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/39.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #39,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/39.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3726,7 +2407,7 @@
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/40.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #40,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/40.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3736,7 +2417,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/41.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #41,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/41.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3746,7 +2427,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/42.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #42,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/42.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3756,7 +2437,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/43.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #43,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/43.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3766,7 +2447,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/44.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #44,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/44.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3776,7 +2457,7 @@
       </c>
       <c r="B46" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/45.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #45,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/45.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3786,7 +2467,7 @@
       </c>
       <c r="B47" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/46.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #46,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/46.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3796,7 +2477,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/47.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #47,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/47.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3806,7 +2487,7 @@
       </c>
       <c r="B49" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/48.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #48,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/48.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3816,7 +2497,7 @@
       </c>
       <c r="B50" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/49.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #49,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/49.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3826,7 +2507,7 @@
       </c>
       <c r="B51" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/50.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #50,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/50.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3836,7 +2517,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/51.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #51,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/51.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3846,7 +2527,7 @@
       </c>
       <c r="B53" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/52.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #52,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/52.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3856,7 +2537,7 @@
       </c>
       <c r="B54" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/53.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #53,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/53.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3866,7 +2547,7 @@
       </c>
       <c r="B55" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/54.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #54,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/54.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3876,7 +2557,7 @@
       </c>
       <c r="B56" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/55.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #55,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/55.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3886,7 +2567,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/56.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #56,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/56.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3896,7 +2577,7 @@
       </c>
       <c r="B58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/57.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #57,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/57.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3906,7 +2587,7 @@
       </c>
       <c r="B59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/58.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #58,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/58.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3916,7 +2597,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/59.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #59,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/59.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +2607,7 @@
       </c>
       <c r="B61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/60.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #60,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/60.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3936,7 +2617,7 @@
       </c>
       <c r="B62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/61.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #61,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/61.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3946,7 +2627,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/62.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #62,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/62.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3956,7 +2637,7 @@
       </c>
       <c r="B64" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/63.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #63,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/63.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,7 +2647,7 @@
       </c>
       <c r="B65" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/64.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #64,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/64.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3975,8 +2656,8 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" ref="B66:B74" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
-        <v>DEBP ENDNOTE CHAPTER 11 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/65.htm,pack-debp-chapter-11</v>
+        <f t="shared" ref="B66:B71" ca="1" si="2">CONCATENATE($B$1," ", $J$1, " #", $A66, ",", TEXT($C$1, "mmmmmmm dd yyyy"), ",", $D$1, "/", $E$1, "/", $F$1, "/", $G$1,"-", $J$1,"/",$A66, ".",$H$1, ",", $I$1, "-", $J$1)</f>
+        <v>DEBP ENDNOTE CHAPTER 12 #65,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/65.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3986,17 +2667,17 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/66.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #66,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/66.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A74" si="3">A67+1</f>
+        <f t="shared" ref="A68:A71" si="3">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/67.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #67,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/67.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -4006,7 +2687,7 @@
       </c>
       <c r="B69" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/68.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #68,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/68.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -4016,7 +2697,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/69.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #69,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/69.htm,pack-debp-chapter-12</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -4026,42 +2707,12 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/70.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="B72" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #71,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/71.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="B73" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #72,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/72.htm,pack-debp-chapter-11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B74" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>DEBP ENDNOTE CHAPTER 11 #73,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-11/73.htm,pack-debp-chapter-11</v>
+        <v>DEBP ENDNOTE CHAPTER 12 #70,April 18 2024,https://htmlpreview.github.io/?https://raw.githubusercontent.com/PacktPublishing/Data-Engineering-Best-Practices/main/Endnotes/chapter-12/70.htm,pack-debp-chapter-12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{68968D13-14DC-481C-A53E-F0199DD9C6CD}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{16425970-E582-43CF-965B-9386FA682BEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4071,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C499C072-DED7-4062-8960-4AF5EC3C5A22}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4785,7 +3436,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B78"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8800,7 +7451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BFB414-1A9D-4ADF-BFBB-0A684113C784}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -8923,8 +7574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E26A37-2E30-42BA-A1DF-2E467DE615AC}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9997,7 +8648,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B57"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12549,7 +11200,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B57"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>